<commit_message>
add Netherlands and Taiwan (and update map, comparisons as a result)
</commit_message>
<xml_diff>
--- a/_comparisonFigure/absolute_comparison_table.xlsx
+++ b/_comparisonFigure/absolute_comparison_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomo/Documents/GitHub/excess-mortality-world/_comparisonFigure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093B57DC-AEB6-874A-AB8D-2FD770683995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CDE843-EBE8-DC42-B4F8-AEBCE6DE1603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="500" windowWidth="30720" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12060" yWindow="8260" windowWidth="30720" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Country</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Rep. Korea</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1041,316 +1044,351 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1">
-        <v>67545</v>
+        <v>339650</v>
       </c>
       <c r="C17" s="1">
-        <v>-2787</v>
+        <v>28495</v>
       </c>
       <c r="D17" s="1">
-        <v>-2566</v>
-      </c>
-      <c r="E17">
-        <v>-872</v>
+        <v>33017</v>
+      </c>
+      <c r="E17" s="1">
+        <v>45500</v>
       </c>
       <c r="F17" s="1">
-        <v>-2677</v>
+        <v>29213</v>
       </c>
       <c r="G17" s="1">
-        <v>-4118</v>
+        <v>17969</v>
       </c>
       <c r="H17" s="1">
-        <v>-5201</v>
+        <v>14175</v>
       </c>
       <c r="I17" s="1">
-        <v>5034795</v>
+        <v>17407606</v>
       </c>
       <c r="J17" s="1">
-        <v>5101593</v>
+        <v>17475445</v>
       </c>
       <c r="K17" s="1">
-        <v>5068194</v>
+        <v>17441526</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
-        <v>82613</v>
+        <v>67545</v>
       </c>
       <c r="C18" s="1">
-        <v>1101</v>
+        <v>-2787</v>
       </c>
       <c r="D18" s="1">
-        <v>1986</v>
+        <v>-2566</v>
       </c>
       <c r="E18">
-        <v>742</v>
-      </c>
-      <c r="F18">
-        <v>-101</v>
+        <v>-872</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-2677</v>
       </c>
       <c r="G18" s="1">
-        <v>-2994</v>
+        <v>-4118</v>
       </c>
       <c r="H18" s="1">
-        <v>-4418</v>
+        <v>-5201</v>
       </c>
       <c r="I18" s="1">
-        <v>5367573</v>
+        <v>5034795</v>
       </c>
       <c r="J18" s="1">
-        <v>5391369</v>
+        <v>5101593</v>
       </c>
       <c r="K18" s="1">
-        <v>5379471</v>
+        <v>5068194</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>248198</v>
+        <v>82613</v>
       </c>
       <c r="C19" s="1">
-        <v>20677</v>
+        <v>1101</v>
       </c>
       <c r="D19" s="1">
-        <v>24530</v>
-      </c>
-      <c r="E19" s="1">
-        <v>40400</v>
-      </c>
-      <c r="F19" s="1">
-        <v>20447</v>
+        <v>1986</v>
+      </c>
+      <c r="E19">
+        <v>742</v>
+      </c>
+      <c r="F19">
+        <v>-101</v>
       </c>
       <c r="G19" s="1">
-        <v>16286</v>
+        <v>-2994</v>
       </c>
       <c r="H19" s="1">
-        <v>10454</v>
+        <v>-4418</v>
       </c>
       <c r="I19" s="1">
-        <v>10315540</v>
+        <v>5367573</v>
       </c>
       <c r="J19" s="1">
-        <v>10315101</v>
+        <v>5391369</v>
       </c>
       <c r="K19" s="1">
-        <v>10315320.5</v>
+        <v>5379471</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>622628</v>
+        <v>248198</v>
       </c>
       <c r="C20" s="1">
-        <v>7529</v>
+        <v>20677</v>
       </c>
       <c r="D20" s="1">
-        <v>6967</v>
+        <v>24530</v>
       </c>
       <c r="E20" s="1">
-        <v>4630</v>
+        <v>40400</v>
       </c>
       <c r="F20" s="1">
-        <v>6288</v>
+        <v>20447</v>
       </c>
       <c r="G20" s="1">
-        <v>-30286</v>
+        <v>16286</v>
       </c>
       <c r="H20" s="1">
-        <v>-62034</v>
+        <v>10454</v>
       </c>
       <c r="I20" s="1">
-        <v>51348579</v>
+        <v>10315540</v>
       </c>
       <c r="J20" s="1">
-        <v>51349116</v>
+        <v>10315101</v>
       </c>
       <c r="K20" s="1">
-        <v>51348847.5</v>
+        <v>10315320.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1">
-        <v>941717</v>
+        <v>622628</v>
       </c>
       <c r="C21" s="1">
-        <v>102991</v>
+        <v>7529</v>
       </c>
       <c r="D21" s="1">
-        <v>115685</v>
+        <v>6967</v>
       </c>
       <c r="E21" s="1">
-        <v>162000</v>
+        <v>4630</v>
       </c>
       <c r="F21" s="1">
-        <v>103937</v>
+        <v>6288</v>
       </c>
       <c r="G21" s="1">
-        <v>68720</v>
+        <v>-30286</v>
       </c>
       <c r="H21" s="1">
-        <v>36310</v>
+        <v>-62034</v>
       </c>
       <c r="I21" s="1">
-        <v>47330878</v>
+        <v>51348579</v>
       </c>
       <c r="J21" s="1">
-        <v>47398697</v>
+        <v>51349116</v>
       </c>
       <c r="K21" s="1">
-        <v>47364787.5</v>
+        <v>51348847.5</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1">
-        <v>190082</v>
+        <v>941717</v>
       </c>
       <c r="C22" s="1">
-        <v>9926</v>
+        <v>102991</v>
       </c>
       <c r="D22" s="1">
-        <v>11976</v>
+        <v>115685</v>
       </c>
       <c r="E22" s="1">
-        <v>18100</v>
+        <v>162000</v>
       </c>
       <c r="F22" s="1">
-        <v>13439</v>
-      </c>
-      <c r="G22">
-        <v>-367</v>
+        <v>103937</v>
+      </c>
+      <c r="G22" s="1">
+        <v>68720</v>
       </c>
       <c r="H22" s="1">
-        <v>-2681</v>
+        <v>36310</v>
       </c>
       <c r="I22" s="1">
-        <v>10327450</v>
+        <v>47330878</v>
       </c>
       <c r="J22" s="1">
-        <v>10379247</v>
+        <v>47398697</v>
       </c>
       <c r="K22" s="1">
-        <v>10353348.5</v>
+        <v>47364787.5</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
-        <v>147387</v>
+        <v>190082</v>
       </c>
       <c r="C23" s="1">
-        <v>11394</v>
+        <v>9926</v>
       </c>
       <c r="D23" s="1">
-        <v>13539</v>
+        <v>11976</v>
       </c>
       <c r="E23" s="1">
-        <v>15500</v>
+        <v>18100</v>
       </c>
       <c r="F23" s="1">
-        <v>8247</v>
-      </c>
-      <c r="G23" s="1">
-        <v>5640</v>
+        <v>13439</v>
+      </c>
+      <c r="G23">
+        <v>-367</v>
       </c>
       <c r="H23" s="1">
-        <v>2256</v>
+        <v>-2681</v>
       </c>
       <c r="I23" s="1">
-        <v>8605887</v>
+        <v>10327450</v>
       </c>
       <c r="J23" s="1">
-        <v>8670243</v>
+        <v>10379247</v>
       </c>
       <c r="K23" s="1">
-        <v>8638065</v>
+        <v>10353348.5</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>1357108</v>
+        <v>147387</v>
       </c>
       <c r="C24" s="1">
-        <v>136795</v>
+        <v>11394</v>
       </c>
       <c r="D24" s="1">
-        <v>148889</v>
+        <v>13539</v>
       </c>
       <c r="E24" s="1">
-        <v>169000</v>
+        <v>15500</v>
       </c>
       <c r="F24" s="1">
-        <v>148897</v>
+        <v>8247</v>
       </c>
       <c r="G24" s="1">
-        <v>87307</v>
+        <v>5640</v>
       </c>
       <c r="H24" s="1">
-        <v>71808</v>
+        <v>2256</v>
       </c>
       <c r="I24" s="1">
-        <v>66939020</v>
+        <v>8605887</v>
       </c>
       <c r="J24" s="1">
-        <v>66930951</v>
+        <v>8670243</v>
       </c>
       <c r="K24" s="1">
-        <v>66934985.5</v>
+        <v>8638065</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1357108</v>
+      </c>
+      <c r="C25" s="1">
+        <v>136795</v>
+      </c>
+      <c r="D25" s="1">
+        <v>148889</v>
+      </c>
+      <c r="E25" s="1">
+        <v>169000</v>
+      </c>
+      <c r="F25" s="1">
+        <v>148897</v>
+      </c>
+      <c r="G25" s="1">
+        <v>87307</v>
+      </c>
+      <c r="H25" s="1">
+        <v>71808</v>
+      </c>
+      <c r="I25" s="1">
+        <v>66939020</v>
+      </c>
+      <c r="J25" s="1">
+        <v>66930951</v>
+      </c>
+      <c r="K25" s="1">
+        <v>66934985.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>6842426</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>961032</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>1017655</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="1">
         <v>1130000</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F26" s="1">
         <v>932458</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G26" s="1">
         <v>871295</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H26" s="1">
         <v>920731</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I26" s="1">
         <v>329791078</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J26" s="1">
         <v>331697950</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K26" s="1">
         <v>330744514</v>
       </c>
     </row>

</xml_diff>